<commit_message>
all functionality added and implemeneted
</commit_message>
<xml_diff>
--- a/book1.xlsx
+++ b/book1.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -28,22 +29,49 @@
     <t xml:space="preserve">Flag</t>
   </si>
   <si>
-    <t xml:space="preserve">Sudhir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swapnil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chinmay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pankaj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shefalli</t>
+    <t xml:space="preserve">sudhirsweet007@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chandramala.k@pacific.co.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hr@webmatrixcorp.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harvinder@elitehrpractices.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dhanashree.m@anlage.co.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harish@idealservices.biz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renu.Jagadish@mindtree.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kavya.ar@peoplefy.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preeti.b.mishra@capgemini.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shambhavi.pandey@lntinfotech.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manjiri.agashe@saviantconsulting.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geeta.m@pacific.co.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pinky.rustagi@nagarro.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prabakaran.sakthivel@careernet.co.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sripriya.mohan@careernet.co.in</t>
   </si>
 </sst>
 </file>
@@ -53,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -74,6 +102,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,8 +153,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,15 +179,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -160,7 +200,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -189,7 +229,35 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sudhirsweet007@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -198,4 +266,56 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>